<commit_message>
commit -m "Atualiza planilha de análise de curto prazo da Embraer"
</commit_message>
<xml_diff>
--- a/planilhas/Analise_Curto_Prazo_Embraer_Completa.xlsx
+++ b/planilhas/Analise_Curto_Prazo_Embraer_Completa.xlsx
@@ -526,7 +526,7 @@
         <v>2.521024850020576</v>
       </c>
       <c r="C2" t="n">
-        <v>1.514304675282405</v>
+        <v>1.501536121434408</v>
       </c>
       <c r="D2" t="n">
         <v>1.111957645262435</v>
@@ -580,7 +580,7 @@
         <v>2.077064802136016</v>
       </c>
       <c r="C3" t="n">
-        <v>1.375041165775489</v>
+        <v>1.363416501871598</v>
       </c>
       <c r="D3" t="n">
         <v>0.9081767724752465</v>
@@ -634,7 +634,7 @@
         <v>1.789310541698855</v>
       </c>
       <c r="C4" t="n">
-        <v>1.065399162577329</v>
+        <v>1.04674837478906</v>
       </c>
       <c r="D4" t="n">
         <v>0.7183916666626953</v>
@@ -688,7 +688,7 @@
         <v>1.651977222909604</v>
       </c>
       <c r="C5" t="n">
-        <v>0.9328475809047825</v>
+        <v>0.9192568588539315</v>
       </c>
       <c r="D5" t="n">
         <v>0.586781461615432</v>
@@ -742,7 +742,7 @@
         <v>1.474636428340116</v>
       </c>
       <c r="C6" t="n">
-        <v>0.8098056475339028</v>
+        <v>0.796505439569714</v>
       </c>
       <c r="D6" t="n">
         <v>0.4987815123960874</v>
@@ -887,7 +887,7 @@
         <v>1.111957645262435</v>
       </c>
       <c r="C2" t="n">
-        <v>1.514304675282405</v>
+        <v>1.501536121434408</v>
       </c>
       <c r="D2" t="n">
         <v>2.521024850020576</v>
@@ -896,7 +896,7 @@
         <v>24465118.7641024</v>
       </c>
       <c r="F2" t="n">
-        <v>24465118.7641024</v>
+        <v>24465118.76410241</v>
       </c>
       <c r="G2" t="n">
         <v>13523549.33623094</v>
@@ -934,7 +934,7 @@
         <v>0.9081767724752465</v>
       </c>
       <c r="C3" t="n">
-        <v>1.375041165775489</v>
+        <v>1.363416501871598</v>
       </c>
       <c r="D3" t="n">
         <v>2.077064802136016</v>
@@ -943,7 +943,7 @@
         <v>19688354.08991013</v>
       </c>
       <c r="F3" t="n">
-        <v>19688354.08991013</v>
+        <v>19688354.08991012</v>
       </c>
       <c r="G3" t="n">
         <v>10096719.09209801</v>
@@ -981,7 +981,7 @@
         <v>0.7183916666626953</v>
       </c>
       <c r="C4" t="n">
-        <v>1.065399162577329</v>
+        <v>1.04674837478906</v>
       </c>
       <c r="D4" t="n">
         <v>1.789310541698855</v>
@@ -990,7 +990,7 @@
         <v>14502530.98141576</v>
       </c>
       <c r="F4" t="n">
-        <v>14502530.98141575</v>
+        <v>14502530.98141576</v>
       </c>
       <c r="G4" t="n">
         <v>9488128.311564919</v>
@@ -1028,7 +1028,7 @@
         <v>0.586781461615432</v>
       </c>
       <c r="C5" t="n">
-        <v>0.9328475809047825</v>
+        <v>0.9192568588539315</v>
       </c>
       <c r="D5" t="n">
         <v>1.651977222909604</v>
@@ -1075,7 +1075,7 @@
         <v>0.4987815123960874</v>
       </c>
       <c r="C6" t="n">
-        <v>0.8098056475339028</v>
+        <v>0.796505439569714</v>
       </c>
       <c r="D6" t="n">
         <v>1.474636428340116</v>
@@ -1125,7 +1125,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T6"/>
+  <dimension ref="A1:U6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1161,72 +1161,77 @@
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
+          <t>AtivoNaoCirculante</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
           <t>AtivoTotal</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>DespesasAntecipadas</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>EmprestimosFinanciamentosCP</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>Fornecedores</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>ObrigacoesTrabalhistas</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>PassivoCirculante</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>PassivoNaoCirculante</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>PatrimonioLiquido</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>ReceitaLiquida</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>CustoMercadoriasVendidas</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>AtivosFinanceirosCP</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>AtivosCiclicosCP</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>PassivosFinanceirosCP</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>PassivosCiclicosCP</t>
-        </is>
-      </c>
-      <c r="T1" s="1" t="inlineStr">
-        <is>
-          <t>AtivoNaoCirculante</t>
         </is>
       </c>
     </row>
@@ -1250,46 +1255,49 @@
         <v>40549746.68045199</v>
       </c>
       <c r="G2" t="n">
+        <v>29141300.63507662</v>
+      </c>
+      <c r="H2" t="n">
         <v>69691047.31552862</v>
       </c>
-      <c r="H2" t="n">
-        <v>0</v>
-      </c>
       <c r="I2" t="n">
+        <v>205377.4376749034</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K2" t="n">
         <v>3326234.649042205</v>
       </c>
-      <c r="J2" t="n">
+      <c r="L2" t="n">
         <v>745801.8544248444</v>
       </c>
-      <c r="K2" t="n">
+      <c r="M2" t="n">
         <v>16084627.91634959</v>
       </c>
-      <c r="L2" t="n">
+      <c r="N2" t="n">
         <v>34305057.82322473</v>
       </c>
-      <c r="M2" t="n">
+      <c r="O2" t="n">
         <v>19301361.5759543</v>
       </c>
-      <c r="N2" t="n">
+      <c r="P2" t="n">
         <v>22827248.50145473</v>
       </c>
-      <c r="O2" t="n">
+      <c r="Q2" t="n">
         <v>-20029943.7315736</v>
       </c>
-      <c r="P2" t="n">
+      <c r="R2" t="n">
         <v>17885424.98278651</v>
       </c>
-      <c r="Q2" t="n">
+      <c r="S2" t="n">
         <v>17595585.83969799</v>
       </c>
-      <c r="R2" t="n">
-        <v>0</v>
-      </c>
-      <c r="S2" t="n">
+      <c r="T2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U2" t="n">
         <v>4072036.503467049</v>
-      </c>
-      <c r="T2" t="n">
-        <v>29141300.63507663</v>
       </c>
     </row>
     <row r="3">
@@ -1312,46 +1320,49 @@
         <v>37967991.53685346</v>
       </c>
       <c r="G3" t="n">
+        <v>27650888.97605425</v>
+      </c>
+      <c r="H3" t="n">
         <v>65618880.5129077</v>
       </c>
-      <c r="H3" t="n">
-        <v>0</v>
-      </c>
       <c r="I3" t="n">
+        <v>212494.6416056913</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K3" t="n">
         <v>3295780.126959153</v>
       </c>
-      <c r="J3" t="n">
+      <c r="L3" t="n">
         <v>723575.5413411085</v>
       </c>
-      <c r="K3" t="n">
+      <c r="M3" t="n">
         <v>18279637.44694333</v>
       </c>
-      <c r="L3" t="n">
+      <c r="N3" t="n">
         <v>29409556.67532437</v>
       </c>
-      <c r="M3" t="n">
+      <c r="O3" t="n">
         <v>17929686.39064</v>
       </c>
-      <c r="N3" t="n">
+      <c r="P3" t="n">
         <v>25011789.94273384</v>
       </c>
-      <c r="O3" t="n">
+      <c r="Q3" t="n">
         <v>-21107048.97528459</v>
       </c>
-      <c r="P3" t="n">
+      <c r="R3" t="n">
         <v>16601142.13858265</v>
       </c>
-      <c r="Q3" t="n">
+      <c r="S3" t="n">
         <v>14116074.76039827</v>
       </c>
-      <c r="R3" t="n">
-        <v>0</v>
-      </c>
-      <c r="S3" t="n">
+      <c r="T3" t="n">
+        <v>0</v>
+      </c>
+      <c r="U3" t="n">
         <v>4019355.668300262</v>
-      </c>
-      <c r="T3" t="n">
-        <v>27650888.97605424</v>
       </c>
     </row>
     <row r="4">
@@ -1374,46 +1385,49 @@
         <v>32876200.42487912</v>
       </c>
       <c r="G4" t="n">
+        <v>25044728.79473388</v>
+      </c>
+      <c r="H4" t="n">
         <v>57920929.21961301</v>
       </c>
-      <c r="H4" t="n">
-        <v>0</v>
-      </c>
       <c r="I4" t="n">
+        <v>342683.40968184</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0</v>
+      </c>
+      <c r="K4" t="n">
         <v>4379905.433120601</v>
       </c>
-      <c r="J4" t="n">
+      <c r="L4" t="n">
         <v>882084.2106615601</v>
       </c>
-      <c r="K4" t="n">
+      <c r="M4" t="n">
         <v>18373669.44346336</v>
       </c>
-      <c r="L4" t="n">
+      <c r="N4" t="n">
         <v>23417345.436912</v>
       </c>
-      <c r="M4" t="n">
+      <c r="O4" t="n">
         <v>16129914.33923764</v>
       </c>
-      <c r="N4" t="n">
+      <c r="P4" t="n">
         <v>24647341.8045608</v>
       </c>
-      <c r="O4" t="n">
+      <c r="Q4" t="n">
         <v>-19696615.91543162</v>
       </c>
-      <c r="P4" t="n">
+      <c r="R4" t="n">
         <v>13199491.01419908</v>
       </c>
-      <c r="Q4" t="n">
+      <c r="S4" t="n">
         <v>14750117.95534708</v>
       </c>
-      <c r="R4" t="n">
-        <v>0</v>
-      </c>
-      <c r="S4" t="n">
+      <c r="T4" t="n">
+        <v>0</v>
+      </c>
+      <c r="U4" t="n">
         <v>5261989.643782161</v>
-      </c>
-      <c r="T4" t="n">
-        <v>25044728.79473389</v>
       </c>
     </row>
     <row r="5">
@@ -1436,46 +1450,49 @@
         <v>30670519.513</v>
       </c>
       <c r="G5" t="n">
+        <v>23942405.2206</v>
+      </c>
+      <c r="H5" t="n">
         <v>54612924.7336</v>
       </c>
-      <c r="H5" t="n">
-        <v>0</v>
-      </c>
       <c r="I5" t="n">
+        <v>252324.6084</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K5" t="n">
         <v>4176279.7472</v>
       </c>
-      <c r="J5" t="n">
+      <c r="L5" t="n">
         <v>1206372.1738</v>
       </c>
-      <c r="K5" t="n">
+      <c r="M5" t="n">
         <v>18565945.7574</v>
       </c>
-      <c r="L5" t="n">
+      <c r="N5" t="n">
         <v>20652951.5502</v>
       </c>
-      <c r="M5" t="n">
+      <c r="O5" t="n">
         <v>15394027.426</v>
       </c>
-      <c r="N5" t="n">
+      <c r="P5" t="n">
         <v>27419853.60827202</v>
       </c>
-      <c r="O5" t="n">
+      <c r="Q5" t="n">
         <v>-22690632.65028139</v>
       </c>
-      <c r="P5" t="n">
+      <c r="R5" t="n">
         <v>10894152.7878</v>
       </c>
-      <c r="Q5" t="n">
+      <c r="S5" t="n">
         <v>14495899.2506</v>
       </c>
-      <c r="R5" t="n">
-        <v>0</v>
-      </c>
-      <c r="S5" t="n">
+      <c r="T5" t="n">
+        <v>0</v>
+      </c>
+      <c r="U5" t="n">
         <v>5382651.921</v>
-      </c>
-      <c r="T5" t="n">
-        <v>23942405.2206</v>
       </c>
     </row>
     <row r="6">
@@ -1498,46 +1515,49 @@
         <v>40326906</v>
       </c>
       <c r="G6" t="n">
+        <v>32892812</v>
+      </c>
+      <c r="H6" t="n">
         <v>73219718</v>
       </c>
-      <c r="H6" t="n">
-        <v>0</v>
-      </c>
       <c r="I6" t="n">
+        <v>363721</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0</v>
+      </c>
+      <c r="K6" t="n">
         <v>6251565</v>
       </c>
-      <c r="J6" t="n">
+      <c r="L6" t="n">
         <v>1055536</v>
       </c>
-      <c r="K6" t="n">
+      <c r="M6" t="n">
         <v>27347016</v>
       </c>
-      <c r="L6" t="n">
+      <c r="N6" t="n">
         <v>25161794</v>
       </c>
-      <c r="M6" t="n">
+      <c r="O6" t="n">
         <v>20710908</v>
       </c>
-      <c r="N6" t="n">
+      <c r="P6" t="n">
         <v>35424174</v>
       </c>
-      <c r="O6" t="n">
+      <c r="Q6" t="n">
         <v>-29041940</v>
       </c>
-      <c r="P6" t="n">
+      <c r="R6" t="n">
         <v>13640186</v>
       </c>
-      <c r="Q6" t="n">
+      <c r="S6" t="n">
         <v>20243028</v>
       </c>
-      <c r="R6" t="n">
-        <v>0</v>
-      </c>
-      <c r="S6" t="n">
+      <c r="T6" t="n">
+        <v>0</v>
+      </c>
+      <c r="U6" t="n">
         <v>7307101</v>
-      </c>
-      <c r="T6" t="n">
-        <v>32892812</v>
       </c>
     </row>
   </sheetData>

</xml_diff>